<commit_message>
Added Password forgot option, added manage connection option,added the UI for manage connection file
</commit_message>
<xml_diff>
--- a/InsertDataScript/demo_file.xlsx
+++ b/InsertDataScript/demo_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t xml:space="preserve">Test Class</t>
   </si>
@@ -46,20 +46,20 @@
     <t xml:space="preserve">Count Verification</t>
   </si>
   <si>
-    <t xml:space="preserve">SourcedbType:postgres;
+    <t xml:space="preserve">sourcedbType:mysql;
 sourceServer:localhost;
-sourcedb:TestDB;
+sourcedb:source_db;
 sourceuser:Acciom_user;
 targetdbType:mysql;
-targetdb:NewTestDB;
+targetdb:dest_db;
 targetServer:localhost;
 targetuser:Acciom_user;</t>
   </si>
   <si>
-    <t xml:space="preserve">Inventory:NewInventory1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@srcqry1:Select count(1) from Inventory where id&gt;10;@targetqry:Select count(1) from NewInventory where id&gt;10;</t>
+    <t xml:space="preserve">src_inventory:dest_inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srcqry:SELECT COUNT( 1)  FROM src_inventory where Company_key &lt;100;targetqry:SELECT COUNT(1) FROM dest_inventory where Company_key &lt;200</t>
   </si>
   <si>
     <t xml:space="preserve">Datavalidation</t>
@@ -68,33 +68,13 @@
     <t xml:space="preserve">Data Validation</t>
   </si>
   <si>
-    <t xml:space="preserve">SourcedbType:sqlserver;
-sourceServer:localhost;
-sourcedb:NewTestDB;
-sourceuser:Acciom_user;
-targetdbType:mysql;
-targetdb:NewTestDB;
-targetServer:localhost;
-targetuser:Acciom_user;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory:NewInventory</t>
-  </si>
-  <si>
     <t xml:space="preserve">DuplicateCheck</t>
   </si>
   <si>
     <t xml:space="preserve">Find Duplicates</t>
   </si>
   <si>
-    <t xml:space="preserve">SourcedbType:mysql;
-sourceServer:localhost;
-sourcedb:TestDB;
-sourceuser:Acciom_user;
-targetdbType:mysql;
-targetdb:NewTestDB;
-targetServer:localhost;
-targetuser:Acciom_user;</t>
+    <t xml:space="preserve">DELETE_FLAG</t>
   </si>
   <si>
     <t xml:space="preserve">NullCheck</t>
@@ -110,9 +90,6 @@
   </si>
   <si>
     <t xml:space="preserve">Duplicate check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@targetqry:SELECT id, count(*) from NewInventory group by id having count(*) &gt;1</t>
   </si>
 </sst>
 </file>
@@ -122,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -158,6 +135,14 @@
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF008080"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -216,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +220,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,8 +305,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,7 +341,7 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="115" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="142" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -371,7 +360,7 @@
       </c>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="116" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="126.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -379,61 +368,65 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="126.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -447,10 +440,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -464,46 +457,46 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="4" customFormat="true" ht="146.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" s="3"/>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AMJ9" s="0"/>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>

<commit_message>
Null Check will show only first 10 rows.
</commit_message>
<xml_diff>
--- a/InsertDataScript/demo_file.xlsx
+++ b/InsertDataScript/demo_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t xml:space="preserve">Test Class</t>
   </si>
@@ -56,7 +56,7 @@
 targetuser:Acciom_user;</t>
   </si>
   <si>
-    <t xml:space="preserve">src_inventory:dest_inventory</t>
+    <t xml:space="preserve">src_inventory1:dest_inventory1</t>
   </si>
   <si>
     <t xml:space="preserve">srcqry:SELECT COUNT( 1)  FROM src_inventory where Company_key &lt;100;targetqry:SELECT COUNT(1) FROM dest_inventory where Company_key &lt;200</t>
@@ -83,10 +83,16 @@
     <t xml:space="preserve">Null Checks</t>
   </si>
   <si>
+    <t xml:space="preserve">src_inventory1:dest_inventory4</t>
+  </si>
+  <si>
     <t xml:space="preserve">DDLCheck</t>
   </si>
   <si>
     <t xml:space="preserve">Schema Compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src_inventory1:dest_inventory5</t>
   </si>
   <si>
     <t xml:space="preserve">Duplicate check</t>
@@ -305,8 +311,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,7 +413,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>15</v>
@@ -417,16 +423,16 @@
     </row>
     <row r="6" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -471,7 +477,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
file upload issue resolved
</commit_message>
<xml_diff>
--- a/InsertDataScript/demo_file.xlsx
+++ b/InsertDataScript/demo_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t xml:space="preserve">Test Class</t>
   </si>
@@ -44,6 +44,28 @@
   </si>
   <si>
     <t xml:space="preserve">Count Verification-custom qry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourcedbType:sqlserver;
+sourceServer:localhost;
+sourcedb:source_db;
+sourceuser:Acciom_user;
+targetdbType:mysql;
+targetdb:dest_db;
+targetServer:localhost;
+targetuser:Acciom_user;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src_inventory1:dest_inventory1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datavalidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Validation</t>
   </si>
   <si>
     <t xml:space="preserve">sourcedbType:mysql;
@@ -56,18 +78,6 @@
 targetuser:Acciom_user;</t>
   </si>
   <si>
-    <t xml:space="preserve">src_inventory1:dest_inventory1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">srcqry:SELECT COUNT( 1)  FROM src_inventory where Company_key &lt;100;targetqry:SELECT COUNT(1) FROM dest_inventory where Company_key &lt;200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datavalidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Validation</t>
-  </si>
-  <si>
     <t xml:space="preserve">DuplicateCheck</t>
   </si>
   <si>
@@ -83,19 +93,22 @@
     <t xml:space="preserve">Null Checks</t>
   </si>
   <si>
+    <t xml:space="preserve">DELETE_FLAG;ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDLCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema Compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate check</t>
+  </si>
+  <si>
     <t xml:space="preserve">DELETE_FLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDLCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schema Compare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count Verification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicate check</t>
   </si>
 </sst>
 </file>
@@ -311,8 +324,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,7 +387,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -385,51 +398,51 @@
     </row>
     <row r="4" s="4" customFormat="true" ht="126.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -443,10 +456,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -463,7 +476,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
@@ -474,32 +487,32 @@
     </row>
     <row r="9" s="4" customFormat="true" ht="146.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3"/>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
changes after integration testing
</commit_message>
<xml_diff>
--- a/InsertDataScript/demo_file.xlsx
+++ b/InsertDataScript/demo_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t xml:space="preserve">Test Class</t>
   </si>
@@ -46,14 +46,14 @@
     <t xml:space="preserve">Count Verification-custom qry</t>
   </si>
   <si>
-    <t xml:space="preserve">sourcedbType:sqlserver;
+    <t xml:space="preserve">sourcedbType:mysql;
 sourceServer:localhost;
 sourcedb:source_db;
-sourceuser:Acciom_user;
+sourceuser:acciom_user;
 targetdbType:mysql;
 targetdb:dest_db;
 targetServer:localhost;
-targetuser:Acciom_user;</t>
+targetuser:acciom_user;</t>
   </si>
   <si>
     <t xml:space="preserve">src_inventory1:dest_inventory1</t>
@@ -68,16 +68,6 @@
     <t xml:space="preserve">Data Validation</t>
   </si>
   <si>
-    <t xml:space="preserve">sourcedbType:mysql;
-sourceServer:localhost;
-sourcedb:source_db;
-sourceuser:Acciom_user;
-targetdbType:mysql;
-targetdb:dest_db;
-targetServer:localhost;
-targetuser:Acciom_user;</t>
-  </si>
-  <si>
     <t xml:space="preserve">DuplicateCheck</t>
   </si>
   <si>
@@ -106,9 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">Duplicate check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELETE_FLAG</t>
   </si>
 </sst>
 </file>
@@ -325,7 +312,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -387,7 +374,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -398,51 +385,51 @@
     </row>
     <row r="4" s="4" customFormat="true" ht="126.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="F5" s="3"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -456,10 +443,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -476,7 +463,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
@@ -487,32 +474,30 @@
     </row>
     <row r="9" s="4" customFormat="true" ht="146.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="3"/>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" s="4" customFormat="true" ht="136.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>

</xml_diff>